<commit_message>
Processed Results - refactorization
</commit_message>
<xml_diff>
--- a/Processed Results/Mi 9T/Cpu/Cpu - Processed.xlsx
+++ b/Processed Results/Mi 9T/Cpu/Cpu - Processed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Mi 9T\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Mi 9T\Cpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB13438-FF3F-4E0D-8779-9CF5507A8148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3B5A54-CC06-4933-8097-64835433F15F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
+    <workbookView xWindow="5340" yWindow="370" windowWidth="9990" windowHeight="9830" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Blad1!$A$2:$A$31</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Blad1!$B$2:$B$31</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$98:$A$187</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$98:$B$187</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Blad1!$A$34:$A$63</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Blad1!$B$33</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Blad1!$B$34:$B$63</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Blad1!$A$66:$A$95</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Blad1!$B$65</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Blad1!$B$66:$B$95</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$66:$A$95</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$65</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Blad1!$B$66:$B$95</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Blad1!$A$34:$A$63</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Blad1!$B$33</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Blad1!$B$34:$B$63</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Blad1!$A$98:$A$187</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Blad1!$B$98:$B$187</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -203,11 +203,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="nl-NL"/>
-              <a:t>Cpu</a:t>
+              <a:t>CPU</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="nl-NL" baseline="0"/>
-              <a:t> factorial - low frequency</a:t>
+              <a:t> - low frequency</a:t>
             </a:r>
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
@@ -831,11 +831,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="nl-NL"/>
-              <a:t>Cpu</a:t>
+              <a:t>CPU </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="nl-NL" baseline="0"/>
-              <a:t> factorial - medium frequency</a:t>
+              <a:t>- medium frequency</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1427,7 +1427,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Cpu factorial</a:t>
+              <a:t>CPU</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -2103,7 +2103,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Cpu factorial - low frequency</cx:v>
+          <cx:v>CPU - low frequency</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -2123,7 +2123,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Cpu factorial - low frequency</a:t>
+            <a:t>CPU - low frequency</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -2214,10 +2214,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2225,7 +2225,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Cpu factorial</cx:v>
+          <cx:v>CPU</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -2245,7 +2245,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Cpu factorial</a:t>
+            <a:t>CPU</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -2335,10 +2335,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2346,7 +2346,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Cpu factorial - medium frequency</cx:v>
+          <cx:v>CPU - medium frequency</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -2366,7 +2366,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Cpu factorial - medium frequency</a:t>
+            <a:t>CPU - medium frequency</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -2376,7 +2376,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3F5A16A3-6E4C-4475-A634-1322A70DC713}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>Medium_frequency</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2463,10 +2463,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2474,7 +2474,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Cpu factorial - high frequency</cx:v>
+          <cx:v>CPU - high frequency</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -2494,7 +2494,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Cpu factorial - high frequency</a:t>
+            <a:t>CPU - high frequency</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -2504,7 +2504,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{138ACD3C-CAEA-4AEF-B3DF-B982F1EA92CC}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>High_frequency</cx:v>
             </cx:txData>
           </cx:tx>
@@ -7198,8 +7198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FE0459-F6C0-45BE-AD60-56F63431C3F0}">
   <dimension ref="A1:E187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>